<commit_message>
<daily>: add 2022-5-24 and add debug 模板 and add vscode 配置
</commit_message>
<xml_diff>
--- a/力扣打卡记录.xlsx
+++ b/力扣打卡记录.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA3C36C2-A195-412E-8E9B-4928A5FF47C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26FD2DF4-F806-42F8-8D0A-90372EC46314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
   <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -156,6 +156,54 @@
   <si>
     <t>2022.5.23</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022.5.24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>剑指offer 数组中重复的数字 （https://leetcode.cn/problems/shu-zu-zhong-zhong-fu-de-shu-zi-lcof/ ）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>剑指offer 二维数组中的查找 （https://leetcode.cn/problems/er-wei-shu-zu-zhong-de-cha-zhao-lcof/ ）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中等</t>
+  </si>
+  <si>
+    <t>提示后通过</t>
+  </si>
+  <si>
+    <t>哈希、算法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>算法、矩阵操作</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.统计数目一般用哈希。2.unordered_map用[]初始化直接有初始值0。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.不要拘泥于固有思想，必须从第一个数字开始查找。2.二维vector如何初始化。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>待巩固</t>
+  </si>
+  <si>
+    <t>unordered_map的使用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vector的初始化与使用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>待学习</t>
   </si>
 </sst>
 </file>
@@ -239,7 +287,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -270,6 +318,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -282,10 +336,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -790,13 +841,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1823,8 +1874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE2C6781-4CF5-40F6-8069-6C29BB48CB57}">
   <dimension ref="A1:M72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1885,7 +1936,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="10" t="s">
         <v>32</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1923,37 +1974,97 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A3" s="1"/>
+      <c r="A3" s="11"/>
       <c r="C3"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C4"/>
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4">
+        <v>30</v>
+      </c>
+      <c r="F4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K4" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A5" s="1"/>
-      <c r="C5"/>
+      <c r="A5" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5">
+        <v>50</v>
+      </c>
+      <c r="F5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J5" t="s">
+        <v>46</v>
+      </c>
+      <c r="K5" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A6" s="1"/>
+      <c r="A6" s="11"/>
       <c r="C6"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A7" s="1"/>
+      <c r="A7" s="11"/>
       <c r="C7"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A8" s="1"/>
+      <c r="A8" s="11"/>
       <c r="C8"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A9" s="1"/>
+      <c r="A9" s="11"/>
       <c r="C9"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A10" s="1"/>
+      <c r="A10" s="11"/>
       <c r="B10" s="7"/>
       <c r="D10" s="6"/>
       <c r="E10" s="2"/>
@@ -1965,7 +2076,7 @@
       <c r="L10" s="6"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A11" s="1"/>
+      <c r="A11" s="11"/>
       <c r="E11" s="2"/>
       <c r="G11" s="9"/>
       <c r="H11" s="2"/>
@@ -1975,7 +2086,7 @@
       <c r="L11" s="6"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A12" s="1"/>
+      <c r="A12" s="11"/>
       <c r="E12" s="2"/>
       <c r="G12" s="9"/>
       <c r="H12" s="2"/>
@@ -1985,7 +2096,7 @@
       <c r="L12" s="6"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A13" s="1"/>
+      <c r="A13" s="11"/>
       <c r="E13" s="2"/>
       <c r="G13" s="9"/>
       <c r="H13" s="2"/>
@@ -1995,7 +2106,7 @@
       <c r="L13" s="6"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A14" s="1"/>
+      <c r="A14" s="11"/>
       <c r="E14" s="2"/>
       <c r="G14" s="9"/>
       <c r="H14" s="2"/>
@@ -2005,7 +2116,7 @@
       <c r="L14" s="6"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A15" s="1"/>
+      <c r="A15" s="11"/>
       <c r="E15" s="2"/>
       <c r="G15" s="9"/>
       <c r="H15" s="2"/>
@@ -2015,7 +2126,7 @@
       <c r="L15" s="6"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A16" s="1"/>
+      <c r="A16" s="11"/>
       <c r="E16" s="2"/>
       <c r="G16" s="9"/>
       <c r="H16" s="2"/>
@@ -2025,7 +2136,7 @@
       <c r="L16" s="6"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A17" s="1"/>
+      <c r="A17" s="11"/>
       <c r="E17" s="2"/>
       <c r="G17" s="9"/>
       <c r="H17" s="2"/>
@@ -2035,7 +2146,7 @@
       <c r="L17" s="6"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A18" s="1"/>
+      <c r="A18" s="11"/>
       <c r="E18" s="2"/>
       <c r="G18" s="9"/>
       <c r="H18" s="2"/>
@@ -2045,7 +2156,7 @@
       <c r="L18" s="6"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A19" s="1"/>
+      <c r="A19" s="11"/>
       <c r="E19" s="2"/>
       <c r="G19" s="9"/>
       <c r="H19" s="2"/>
@@ -2055,7 +2166,7 @@
       <c r="L19" s="6"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A20" s="1"/>
+      <c r="A20" s="11"/>
       <c r="E20" s="2"/>
       <c r="G20" s="9"/>
       <c r="H20" s="2"/>
@@ -2065,7 +2176,7 @@
       <c r="L20" s="6"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A21" s="1"/>
+      <c r="A21" s="11"/>
       <c r="E21" s="2"/>
       <c r="G21" s="9"/>
       <c r="H21" s="2"/>
@@ -2075,7 +2186,7 @@
       <c r="L21" s="6"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A22" s="1"/>
+      <c r="A22" s="11"/>
       <c r="E22" s="2"/>
       <c r="G22" s="9"/>
       <c r="H22" s="2"/>
@@ -2085,7 +2196,7 @@
       <c r="L22" s="6"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A23" s="1"/>
+      <c r="A23" s="11"/>
       <c r="E23" s="2"/>
       <c r="G23" s="9"/>
       <c r="H23" s="2"/>
@@ -2095,7 +2206,7 @@
       <c r="L23" s="6"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A24" s="1"/>
+      <c r="A24" s="11"/>
       <c r="E24" s="2"/>
       <c r="G24" s="9"/>
       <c r="H24" s="2"/>
@@ -2105,7 +2216,7 @@
       <c r="L24" s="6"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A25" s="1"/>
+      <c r="A25" s="11"/>
       <c r="E25" s="2"/>
       <c r="G25" s="9"/>
       <c r="H25" s="2"/>
@@ -2115,7 +2226,7 @@
       <c r="L25" s="6"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A26" s="1"/>
+      <c r="A26" s="11"/>
       <c r="E26" s="2"/>
       <c r="G26" s="9"/>
       <c r="H26" s="2"/>
@@ -2125,7 +2236,7 @@
       <c r="L26" s="6"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A27" s="1"/>
+      <c r="A27" s="11"/>
       <c r="E27" s="2"/>
       <c r="G27" s="9"/>
       <c r="H27" s="2"/>
@@ -2135,7 +2246,7 @@
       <c r="L27" s="6"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A28" s="1"/>
+      <c r="A28" s="11"/>
       <c r="E28" s="2"/>
       <c r="G28" s="9"/>
       <c r="H28" s="2"/>
@@ -2145,7 +2256,7 @@
       <c r="L28" s="6"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A29" s="1"/>
+      <c r="A29" s="11"/>
       <c r="E29" s="2"/>
       <c r="G29" s="9"/>
       <c r="H29" s="2"/>
@@ -2155,7 +2266,7 @@
       <c r="L29" s="6"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A30" s="1"/>
+      <c r="A30" s="11"/>
       <c r="E30" s="2"/>
       <c r="G30" s="9"/>
       <c r="H30" s="2"/>
@@ -2165,7 +2276,7 @@
       <c r="L30" s="6"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A31" s="1"/>
+      <c r="A31" s="11"/>
       <c r="E31" s="2"/>
       <c r="G31" s="9"/>
       <c r="H31" s="2"/>
@@ -2175,7 +2286,7 @@
       <c r="L31" s="6"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A32" s="1"/>
+      <c r="A32" s="11"/>
       <c r="E32" s="2"/>
       <c r="G32" s="9"/>
       <c r="H32" s="2"/>
@@ -2185,17 +2296,20 @@
       <c r="L32" s="6"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A33" s="1"/>
+      <c r="A33" s="11"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A34" s="16"/>
     </row>
     <row r="35" spans="1:7" ht="22.15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="10" t="s">
+      <c r="A35" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B35" s="10"/>
-      <c r="D35" s="10" t="s">
+      <c r="B35" s="12"/>
+      <c r="D35" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E35" s="10"/>
+      <c r="E35" s="12"/>
       <c r="G35" s="4" t="s">
         <v>19</v>
       </c>
@@ -2206,18 +2320,18 @@
       </c>
       <c r="B36">
         <f>COUNTIF(C2:C32,"简单")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E36">
         <f>COUNTIF(D2:D32,"通过")</f>
-        <v>1</v>
-      </c>
-      <c r="G36" s="11">
+        <v>2</v>
+      </c>
+      <c r="G36" s="13">
         <f>ROUND(AVERAGE(E2:E32), 0)</f>
-        <v>14</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.15">
@@ -2226,7 +2340,7 @@
       </c>
       <c r="B37">
         <f>COUNTIF(C2:C32,"中等")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>13</v>
@@ -2235,7 +2349,7 @@
         <f>COUNTIF(D2:D32,"超时通过")</f>
         <v>0</v>
       </c>
-      <c r="G37" s="11"/>
+      <c r="G37" s="13"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
@@ -2250,9 +2364,9 @@
       </c>
       <c r="E38">
         <f>COUNTIF(D2:D32,"提示后通过")</f>
-        <v>0</v>
-      </c>
-      <c r="G38" s="11"/>
+        <v>1</v>
+      </c>
+      <c r="G38" s="13"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A39" s="1"/>
@@ -2263,55 +2377,55 @@
         <f>COUNTIF(D2:D32,"CV-未通过")</f>
         <v>0</v>
       </c>
-      <c r="G39" s="11"/>
+      <c r="G39" s="13"/>
     </row>
     <row r="40" spans="1:7" ht="25.15" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="41" spans="1:7" ht="26.45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="12" t="s">
+      <c r="A41" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B41" s="12"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="12"/>
+      <c r="B41" s="14"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A42" s="13"/>
-      <c r="B42" s="13"/>
-      <c r="C42" s="13"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13"/>
+      <c r="A42" s="15"/>
+      <c r="B42" s="15"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="15"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="15"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A43" s="13"/>
-      <c r="B43" s="13"/>
-      <c r="C43" s="13"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="13"/>
-      <c r="F43" s="13"/>
-      <c r="G43" s="13"/>
+      <c r="A43" s="15"/>
+      <c r="B43" s="15"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="15"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A44" s="13"/>
-      <c r="B44" s="13"/>
-      <c r="C44" s="13"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="13"/>
+      <c r="A44" s="15"/>
+      <c r="B44" s="15"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="15"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="15"/>
+      <c r="G44" s="15"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A45" s="13"/>
-      <c r="B45" s="13"/>
-      <c r="C45" s="13"/>
-      <c r="D45" s="13"/>
-      <c r="E45" s="13"/>
-      <c r="F45" s="13"/>
-      <c r="G45" s="13"/>
+      <c r="A45" s="15"/>
+      <c r="B45" s="15"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="15"/>
+      <c r="F45" s="15"/>
+      <c r="G45" s="15"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A46" s="1"/>

</xml_diff>

<commit_message>
<daily>: add 2022-05-25 daily`
</commit_message>
<xml_diff>
--- a/力扣打卡记录.xlsx
+++ b/力扣打卡记录.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26FD2DF4-F806-42F8-8D0A-90372EC46314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B188C307-F81E-4802-A1E0-04AFDDFAB7A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="52">
   <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -204,6 +204,26 @@
   </si>
   <si>
     <t>待学习</t>
+  </si>
+  <si>
+    <t>2022.5.25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>剑指offer 替换空格（https://leetcode.cn/problems/ti-huan-kong-ge-lcof/）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>字符串</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.字符串初始化等。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string的使用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -324,6 +344,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -335,9 +358,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -841,7 +861,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1874,8 +1894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE2C6781-4CF5-40F6-8069-6C29BB48CB57}">
   <dimension ref="A1:M72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2048,8 +2068,39 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A6" s="11"/>
-      <c r="C6"/>
+      <c r="A6" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6">
+        <v>20</v>
+      </c>
+      <c r="F6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" t="s">
+        <v>43</v>
+      </c>
+      <c r="I6" t="s">
+        <v>51</v>
+      </c>
+      <c r="J6" t="s">
+        <v>46</v>
+      </c>
+      <c r="K6" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A7" s="11"/>
@@ -2299,17 +2350,17 @@
       <c r="A33" s="11"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A34" s="16"/>
+      <c r="A34" s="12"/>
     </row>
     <row r="35" spans="1:7" ht="22.15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="12" t="s">
+      <c r="A35" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B35" s="12"/>
-      <c r="D35" s="12" t="s">
+      <c r="B35" s="13"/>
+      <c r="D35" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E35" s="12"/>
+      <c r="E35" s="13"/>
       <c r="G35" s="4" t="s">
         <v>19</v>
       </c>
@@ -2320,18 +2371,18 @@
       </c>
       <c r="B36">
         <f>COUNTIF(C2:C32,"简单")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E36">
         <f>COUNTIF(D2:D32,"通过")</f>
-        <v>2</v>
-      </c>
-      <c r="G36" s="13">
+        <v>3</v>
+      </c>
+      <c r="G36" s="14">
         <f>ROUND(AVERAGE(E2:E32), 0)</f>
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.15">
@@ -2349,7 +2400,7 @@
         <f>COUNTIF(D2:D32,"超时通过")</f>
         <v>0</v>
       </c>
-      <c r="G37" s="13"/>
+      <c r="G37" s="14"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
@@ -2366,7 +2417,7 @@
         <f>COUNTIF(D2:D32,"提示后通过")</f>
         <v>1</v>
       </c>
-      <c r="G38" s="13"/>
+      <c r="G38" s="14"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A39" s="1"/>
@@ -2377,55 +2428,55 @@
         <f>COUNTIF(D2:D32,"CV-未通过")</f>
         <v>0</v>
       </c>
-      <c r="G39" s="13"/>
+      <c r="G39" s="14"/>
     </row>
     <row r="40" spans="1:7" ht="25.15" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="41" spans="1:7" ht="26.45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="14" t="s">
+      <c r="A41" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B41" s="14"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="15"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A42" s="15"/>
-      <c r="B42" s="15"/>
-      <c r="C42" s="15"/>
-      <c r="D42" s="15"/>
-      <c r="E42" s="15"/>
-      <c r="F42" s="15"/>
-      <c r="G42" s="15"/>
+      <c r="A42" s="16"/>
+      <c r="B42" s="16"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A43" s="15"/>
-      <c r="B43" s="15"/>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15"/>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15"/>
-      <c r="G43" s="15"/>
+      <c r="A43" s="16"/>
+      <c r="B43" s="16"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="16"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A44" s="15"/>
-      <c r="B44" s="15"/>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15"/>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15"/>
-      <c r="G44" s="15"/>
+      <c r="A44" s="16"/>
+      <c r="B44" s="16"/>
+      <c r="C44" s="16"/>
+      <c r="D44" s="16"/>
+      <c r="E44" s="16"/>
+      <c r="F44" s="16"/>
+      <c r="G44" s="16"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A45" s="15"/>
-      <c r="B45" s="15"/>
-      <c r="C45" s="15"/>
-      <c r="D45" s="15"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="15"/>
-      <c r="G45" s="15"/>
+      <c r="A45" s="16"/>
+      <c r="B45" s="16"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="16"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="16"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A46" s="1"/>

</xml_diff>